<commit_message>
changing headers and data
</commit_message>
<xml_diff>
--- a/EleccionesPresidenciales2020.xlsx
+++ b/EleccionesPresidenciales2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QIS12\Documents\Vampy\DiplomadoPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D983499-9C0A-4B6C-81FE-60F983429CD0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1ABEBE4-F9B6-4110-8E5F-B74A875F88D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{32652137-F999-40B8-AA49-DDF96E90B877}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <t>Presidentes</t>
   </si>
   <si>
-    <t>#Votos</t>
+    <t>Voto</t>
   </si>
 </sst>
 </file>
@@ -83,7 +83,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,50 +398,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F56A71-CB95-4FCF-9BC6-F88FDF9CC92D}">
-  <dimension ref="D5:E8"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
-        <v>0.433</v>
+      <c r="B2" s="1">
+        <f>0.433*100</f>
+        <v>43.3</v>
       </c>
     </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
-        <v>0.30199999999999999</v>
+      <c r="B3" s="1">
+        <f>0.3028*100</f>
+        <v>30.28</v>
       </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="1">
-        <v>0.153</v>
+      <c r="B4" s="1">
+        <f>0.153*100</f>
+        <v>15.299999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding name of the sheet
</commit_message>
<xml_diff>
--- a/EleccionesPresidenciales2020.xlsx
+++ b/EleccionesPresidenciales2020.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QIS12\Documents\Vampy\DiplomadoPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1ABEBE4-F9B6-4110-8E5F-B74A875F88D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD8F5B8-F2F9-42A8-90BB-134F6B6A088C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{32652137-F999-40B8-AA49-DDF96E90B877}"/>
+    <workbookView xWindow="2790" yWindow="1860" windowWidth="17310" windowHeight="9810" xr2:uid="{32652137-F999-40B8-AA49-DDF96E90B877}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="EleccionesPresidenciales2020" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>